<commit_message>
Calculo de defectos V1
</commit_message>
<xml_diff>
--- a/03_Parcial3/Metricas/Taller 1_G3ACSW.xlsx
+++ b/03_Parcial3/Metricas/Taller 1_G3ACSW.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>EL TAMAÑO DEL PRODUCTO</t>
   </si>
@@ -181,7 +181,13 @@
     <t xml:space="preserve">Estimado </t>
   </si>
   <si>
+    <t xml:space="preserve">Cálculo de defectos </t>
+  </si>
+  <si>
     <t>Tabla 15,1 Estimación de Defectos</t>
+  </si>
+  <si>
+    <t>Jenny Ruiz</t>
   </si>
   <si>
     <t xml:space="preserve">Numero de programas </t>
@@ -388,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -485,11 +491,20 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -499,10 +514,10 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -6145,8 +6160,8 @@
   <sheetData>
     <row r="2">
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
+      <c r="C2" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -6154,8 +6169,8 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3">
-      <c r="B3" s="38" t="s">
-        <v>55</v>
+      <c r="B3" s="39" t="s">
+        <v>56</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -6173,13 +6188,13 @@
       <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>5</v>
+      <c r="E4" s="40" t="s">
+        <v>57</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="41">
         <v>45698.0</v>
       </c>
     </row>
@@ -6216,9 +6231,7 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8">
-      <c r="B8" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="42"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -6226,366 +6239,363 @@
       <c r="G8" s="4"/>
     </row>
     <row r="10">
-      <c r="B10" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="40" t="s">
+      <c r="B10" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="40" t="s">
+      <c r="C10" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="43" t="s">
         <v>58</v>
       </c>
+      <c r="H10" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11">
-      <c r="B11" s="41">
+      <c r="B11" s="44">
         <v>1.0</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="43">
         <v>5.0</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="45">
         <f>'Estimacion 6.2'!F14</f>
         <v>31</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G11" s="44">
         <v>1.0</v>
       </c>
-      <c r="H11" s="40">
+      <c r="H11" s="43">
         <v>3.0</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="43">
         <v>28.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="41">
+      <c r="B12" s="44">
         <v>2.0</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="43">
         <v>3.0</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="45">
         <f>'Estimacion 6.2'!F15</f>
         <v>5</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="44">
         <v>2.0</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="43">
         <v>1.0</v>
       </c>
-      <c r="I12" s="40">
+      <c r="I12" s="43">
         <v>10.0</v>
       </c>
-      <c r="K12" s="43">
-        <v>1000.0</v>
-      </c>
     </row>
     <row r="13">
-      <c r="B13" s="41">
+      <c r="B13" s="44">
         <v>3.0</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="43">
         <v>1.0</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="45">
         <f>'Estimacion 6.2'!F16</f>
         <v>6</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="44">
         <v>3.0</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="43">
         <v>2.0</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="43">
         <v>15.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="41">
+      <c r="B14" s="44">
         <v>4.0</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="43">
         <v>8.0</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="45">
         <f>'Estimacion 6.2'!F17</f>
         <v>20</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="44">
         <v>4.0</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H14" s="43">
         <v>4.0</v>
       </c>
-      <c r="I14" s="40">
+      <c r="I14" s="43">
         <v>8.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="41">
+      <c r="B15" s="44">
         <v>5.0</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="43">
         <v>10.0</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="45">
         <f>'Estimacion 6.2'!F18</f>
         <v>38</v>
       </c>
-      <c r="G15" s="41">
+      <c r="G15" s="44">
         <v>5.0</v>
       </c>
-      <c r="H15" s="40">
+      <c r="H15" s="43">
         <v>4.0</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I15" s="43">
         <v>25.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="41">
+      <c r="B16" s="44">
         <v>6.0</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="43">
         <v>8.0</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="45">
         <f>'Estimacion 6.2'!F20</f>
         <v>30</v>
       </c>
-      <c r="G16" s="41">
+      <c r="G16" s="44">
         <v>6.0</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="43">
         <v>2.0</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="43">
         <v>20.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="41">
+      <c r="B17" s="44">
         <v>7.0</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="43">
         <v>11.0</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="45">
         <f>'Estimacion 6.2'!F21</f>
         <v>26</v>
       </c>
-      <c r="G17" s="41">
+      <c r="G17" s="44">
         <v>7.0</v>
       </c>
-      <c r="H17" s="40">
+      <c r="H17" s="43">
         <v>5.0</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="43">
         <v>50.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="41">
+      <c r="B18" s="44">
         <v>8.0</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="43">
         <v>1.0</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="45">
         <f>'Estimacion 6.2'!F22</f>
         <v>16</v>
       </c>
-      <c r="G18" s="41">
+      <c r="G18" s="44">
         <v>8.0</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="43">
         <v>2.0</v>
       </c>
-      <c r="I18" s="40">
+      <c r="I18" s="43">
         <v>16.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="41">
+      <c r="B19" s="44">
         <v>9.0</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="43">
         <v>1.0</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="45">
         <f>'Estimacion 6.2'!F23</f>
         <v>12</v>
       </c>
-      <c r="G19" s="41">
+      <c r="G19" s="44">
         <v>9.0</v>
       </c>
-      <c r="H19" s="40">
+      <c r="H19" s="43">
         <v>1.0</v>
       </c>
-      <c r="I19" s="40">
+      <c r="I19" s="43">
         <v>18.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="41">
+      <c r="B20" s="44">
         <v>10.0</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="43">
         <v>6.0</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="45">
         <f>'Estimacion 6.2'!F24</f>
         <v>28</v>
       </c>
-      <c r="G20" s="41">
+      <c r="G20" s="44">
         <v>10.0</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="43">
         <v>6.0</v>
       </c>
-      <c r="I20" s="40">
+      <c r="I20" s="43">
         <v>9.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="41">
+      <c r="B21" s="44">
         <v>11.0</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C21" s="43">
         <v>10.0</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="45">
         <f>'Estimacion 6.2'!F25</f>
         <v>64</v>
       </c>
-      <c r="G21" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="40">
+      <c r="G21" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="43">
         <f t="shared" ref="H21:I21" si="1">SUM(H11:H20)</f>
         <v>30</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="45">
         <f t="shared" si="1"/>
         <v>199</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="41">
+      <c r="B22" s="44">
         <v>12.0</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="43">
         <v>1.0</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="45">
         <f>'Estimacion 6.2'!F26</f>
         <v>8</v>
       </c>
-      <c r="G22" s="44"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="45" t="str">
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48" t="str">
         <f>'Estimacion 6.2'!K26</f>
         <v/>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="41">
+      <c r="B23" s="44">
         <v>13.0</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="43">
         <v>9.0</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="45">
         <f>'Estimacion 6.2'!F27</f>
         <v>45</v>
       </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="45" t="str">
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48" t="str">
         <f>'Estimacion 6.2'!K27</f>
         <v/>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="42">
+      <c r="B24" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="45">
         <f>SUM(C11+C12+C13+C14+C15+C16+C17+C18+C19+C20+C21+C22+C23)</f>
         <v>74</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="45">
         <f>SUM(D11:D23)</f>
         <v>329</v>
       </c>
     </row>
     <row r="25">
-      <c r="G25" s="46" t="s">
-        <v>60</v>
+      <c r="G25" s="49" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27">
-      <c r="H27" s="43" t="s">
-        <v>61</v>
+      <c r="H27" s="47" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="46" t="s">
-        <v>62</v>
+      <c r="B28" s="49" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="47">
+      <c r="B30" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="50">
         <f>1000*(C24)/(D24)</f>
         <v>224.9240122</v>
       </c>
-      <c r="D30" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="H30" s="43" t="s">
+      <c r="D30" s="47" t="s">
         <v>66</v>
       </c>
+      <c r="G30" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="47" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="31">
-      <c r="C31" s="47"/>
+      <c r="C31" s="50"/>
     </row>
     <row r="32">
-      <c r="H32" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="I32" s="47">
+      <c r="H32" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="I32" s="50">
         <f>(I21*C30)/1000</f>
         <v>44.75987842</v>
       </c>
-      <c r="J32" s="43" t="s">
-        <v>64</v>
+      <c r="J32" s="47" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35">
-      <c r="G35" s="43" t="s">
-        <v>68</v>
+      <c r="G35" s="47" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="36">
-      <c r="H36" s="43" t="s">
-        <v>69</v>
+      <c r="H36" s="47" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -6601,9 +6611,6 @@
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="G4:G5"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B8"/>
-  </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>